<commit_message>
Add further test cases and replaced explicit waits with implicit waits.
</commit_message>
<xml_diff>
--- a/src/test/java/com/seopa/tests/automated/test/cases/SimpleCarJourney01.xlsx
+++ b/src/test/java/com/seopa/tests/automated/test/cases/SimpleCarJourney01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickmcparland/java/selenium_tests/src/test/java/com/seopa/tests/automated/test/cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.mcparland\Documents\selenium_tests\src\test\java\com\seopa\tests\automated\test\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="636" yWindow="1176" windowWidth="28164" windowHeight="16884" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="129">
   <si>
     <t>Element Type</t>
   </si>
@@ -511,12 +511,18 @@
   <si>
     <t xml:space="preserve">we are currently searching </t>
   </si>
+  <si>
+    <t>About you</t>
+  </si>
+  <si>
+    <t>found_address</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1095,19 +1101,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="8" customWidth="1"/>
-    <col min="2" max="8" width="20.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="28.296875" style="8" customWidth="1"/>
+    <col min="2" max="8" width="20.296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="26.4">
       <c r="A1" s="5" t="s">
         <v>97</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="31.2">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1153,7 +1159,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1179,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -1195,7 +1201,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1217,7 +1223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -1281,7 +1287,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="46.8">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1301,7 +1307,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="46.8">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1321,7 +1327,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="46.8">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1341,7 +1347,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="31.2">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -1361,7 +1367,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="62.4">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -1381,7 +1387,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -1401,7 +1407,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -1417,11 +1423,15 @@
       <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="31.95" customHeight="1">
       <c r="A16" s="7"/>
       <c r="C16" s="19" t="s">
         <v>63</v>
@@ -1432,7 +1442,7 @@
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="31.95" customHeight="1">
       <c r="A17" s="7"/>
       <c r="C17" s="16" t="s">
         <v>50</v>
@@ -1443,7 +1453,7 @@
       <c r="G17" s="17"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="31.2">
       <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1485,7 +1495,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="7" t="s">
         <v>64</v>
       </c>
@@ -1505,7 +1515,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
@@ -1525,7 +1535,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
@@ -1545,7 +1555,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
@@ -1565,7 +1575,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
@@ -1585,7 +1595,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16.2">
       <c r="A25" s="7" t="s">
         <v>53</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="16.2">
       <c r="A26" s="7" t="s">
         <v>56</v>
       </c>
@@ -1627,7 +1637,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="31.2">
       <c r="A27" s="7" t="s">
         <v>58</v>
       </c>
@@ -1647,7 +1657,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="16.2">
       <c r="A28" s="7" t="s">
         <v>60</v>
       </c>
@@ -1667,7 +1677,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="16.2">
       <c r="A29" s="7" t="s">
         <v>61</v>
       </c>
@@ -1687,431 +1697,431 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="16.2">
       <c r="A30" s="7" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>69</v>
+        <v>6</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="46.8">
       <c r="A31" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.2">
+      <c r="A32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+    <row r="33" spans="1:8">
+      <c r="A33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="13" t="s">
+      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E33" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="31.2">
+      <c r="A34" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="B34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16.2">
       <c r="A35" s="7" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="C36" s="16" t="s">
+      <c r="H35" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="31.95" customHeight="1">
+      <c r="A37" s="7"/>
+      <c r="C37" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="13" t="s">
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>84</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="13" t="s">
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:8">
+      <c r="A40" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="13" t="s">
+      <c r="B40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="31.2">
       <c r="A41" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>91</v>
+        <v>25</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="7" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="C44" s="16" t="s">
+      <c r="H43" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" ht="31.95" customHeight="1">
+      <c r="A45" s="7"/>
+      <c r="C45" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="18"/>
-    </row>
-    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="1:8" ht="16.2">
+      <c r="A46" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="14" t="s">
+      <c r="B46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" ht="48" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" ht="46.8">
       <c r="A47" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>107</v>
+      <c r="C47" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H47" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B49" s="9" t="s">
+    <row r="49" spans="1:8">
+      <c r="A49" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
-        <v>114</v>
+      <c r="E49" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>67</v>
@@ -2123,15 +2133,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>67</v>
@@ -2143,132 +2153,148 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E53" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="H54" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+    <row r="55" spans="1:8">
+      <c r="A55" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="7"/>
-      <c r="C55" s="16" t="s">
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" ht="31.95" customHeight="1">
+      <c r="A56" s="7"/>
+      <c r="C56" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="18"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="13" t="s">
+      <c r="B57" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D57" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E57" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
+    <row r="58" spans="1:8">
+      <c r="A58" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="9"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="9"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="9"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="9"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="9"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="9"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="9"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" s="9"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C55:H55"/>
+    <mergeCell ref="C56:H56"/>
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C45:H45"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E32" r:id="rId1"/>
+    <hyperlink ref="E33" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2283,9 +2309,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="46.8">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>

</xml_diff>